<commit_message>
logboek bijgewerkt van iedereen
</commit_message>
<xml_diff>
--- a/Documentatie/logboek-sprint1.xlsx
+++ b/Documentatie/logboek-sprint1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -47,6 +47,45 @@
   </si>
   <si>
     <t>Burndown Chart gemaakt</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Animatie van het logo</t>
+  </si>
+  <si>
+    <t>Robert, Jesse</t>
+  </si>
+  <si>
+    <t>Schetsen op papier van de game</t>
+  </si>
+  <si>
+    <t>HD</t>
+  </si>
+  <si>
+    <t>Jordy</t>
+  </si>
+  <si>
+    <t>Use case diagrammen</t>
+  </si>
+  <si>
+    <t>Quincy</t>
+  </si>
+  <si>
+    <t>Wireframes</t>
+  </si>
+  <si>
+    <t>Dean</t>
+  </si>
+  <si>
+    <t>HTML en CSS van de homepage</t>
+  </si>
+  <si>
+    <t>Slawek</t>
+  </si>
+  <si>
+    <t>verzinnen van de slagzin en de header</t>
   </si>
 </sst>
 </file>
@@ -530,7 +569,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +577,7 @@
     <col min="2" max="2" width="23.85546875" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" style="17" bestFit="1" customWidth="1"/>
   </cols>
@@ -626,21 +665,129 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="15">
+        <v>41964</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="16">
+        <v>1001</v>
+      </c>
+      <c r="G6" s="17">
+        <v>13</v>
+      </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="15">
+        <v>41964</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="16">
+        <v>1028</v>
+      </c>
+      <c r="G7" s="17">
+        <v>40</v>
+      </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="15">
+        <v>41964</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1010</v>
+      </c>
+      <c r="G8" s="17">
+        <v>13</v>
+      </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="15">
+        <v>41964</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="16">
+        <v>1006</v>
+      </c>
+      <c r="G9" s="17">
+        <v>20</v>
+      </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="15">
+        <v>41964</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1004</v>
+      </c>
+      <c r="G10" s="17">
+        <v>20</v>
+      </c>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="15">
+        <v>41964</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="16">
+        <v>1003</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0.5</v>
+      </c>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>